<commit_message>
Built in cases modified
Built in case studies are modified based on the new structure of the sets and parameters
</commit_message>
<xml_diff>
--- a/examples/Utopia1_operation_multi_node/parameters/parameters_connections.xlsx
+++ b/examples/Utopia1_operation_multi_node/parameters/parameters_connections.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\negar\Documents\GitHub\hypatia\Examples\Utopia1_operation_multi_node\parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/negarnamazifard/Documents/GitHub/Hypatia_SESAM/test/parameters_new/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837C97B2-F4CA-7641-9516-154D005107C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="18" windowWidth="16098" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="F_OM" sheetId="1" r:id="rId1"/>
-    <sheet name="V_OM" sheetId="2" r:id="rId2"/>
-    <sheet name="Residual_capacity" sheetId="3" r:id="rId3"/>
-    <sheet name="Capacity_factor_line" sheetId="4" r:id="rId4"/>
-    <sheet name="Line_efficiency" sheetId="5" r:id="rId5"/>
-    <sheet name="AnnualProd_perunit_capacity" sheetId="6" r:id="rId6"/>
+    <sheet name="V_OM" sheetId="1" r:id="rId1"/>
+    <sheet name="F_OM" sheetId="2" r:id="rId2"/>
+    <sheet name="Line_efficiency" sheetId="3" r:id="rId3"/>
+    <sheet name="AnnualProd_perunit_capacity" sheetId="4" r:id="rId4"/>
+    <sheet name="Residual_capacity" sheetId="5" r:id="rId5"/>
+    <sheet name="Capacity_factor_line" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -65,8 +66,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +79,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -126,6 +134,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,6 +228,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -254,6 +280,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -429,19 +472,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="19.3125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +493,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -473,12 +513,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -486,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1.3156000000000001</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -507,19 +547,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="16.578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +566,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -551,12 +586,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -564,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1.3156000000000001</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -585,16 +620,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +641,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -626,29 +661,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>40000</v>
+        <v>0.8</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -660,16 +695,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +716,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -701,28 +736,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>8760</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -735,16 +770,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,7 +791,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -776,29 +811,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.8</v>
+        <v>40000</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -810,16 +845,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -831,7 +866,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -851,20 +886,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>8760</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>

</xml_diff>

<commit_message>
modify optimization module for the new trade structure
@mohammadamint post-process still need to be modified

Manual unit-test based on the comparison of similar case studies have been implemented
</commit_message>
<xml_diff>
--- a/examples/Utopia1_operation_multi_node/parameters/parameters_connections.xlsx
+++ b/examples/Utopia1_operation_multi_node/parameters/parameters_connections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/negarnamazifard/Documents/GitHub/Hypatia_SESAM/test/parameters_new/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vitoresearch-my.sharepoint.com/personal/negar_namazifard_vito_be/Documents/Documents/GitHub/Hypatia/examples/Utopia1_operation_multi_node/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837C97B2-F4CA-7641-9516-154D005107C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{837C97B2-F4CA-7641-9516-154D005107C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{06441DE2-DA56-4ADB-9A37-D73AECF0B26C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V_OM" sheetId="1" r:id="rId1"/>
@@ -131,10 +131,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,25 +475,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -513,12 +516,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -552,21 +555,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -586,12 +589,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -627,21 +630,21 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -661,12 +664,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -702,21 +705,21 @@
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,28 +739,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
         <v>8760</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
         <v>1</v>
       </c>
     </row>
@@ -777,21 +780,21 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -811,12 +814,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -848,25 +851,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -886,12 +889,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>